<commit_message>
Testing stuff updated; +1 fist bug created
Signed-off-by: muellers <stefan.mueller@vol.at>
</commit_message>
<xml_diff>
--- a/testing/Template_TestCases.xlsx
+++ b/testing/Template_TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Testobjekt:</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Tester123</t>
+  </si>
+  <si>
+    <t>Testdaten</t>
+  </si>
+  <si>
+    <t>Kunde anlegen</t>
+  </si>
+  <si>
+    <t>....</t>
+  </si>
+  <si>
+    <t>aus Bug-Liste</t>
   </si>
 </sst>
 </file>
@@ -161,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -169,11 +181,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -204,112 +231,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -603,24 +524,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -631,8 +553,9 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -643,27 +566,30 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="T4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="G4" s="4"/>
+      <c r="U4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -671,138 +597,667 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21" ht="30">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>6</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>7</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>8</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>9</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>10</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>11</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>12</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>13</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>14</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="10"/>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="10"/>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="10"/>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="10"/>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="10"/>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="10"/>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="10"/>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="C77" s="9"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="C78" s="9"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="C79" s="9"/>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="C80" s="9"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F6:F48">
+  <conditionalFormatting sqref="G6:G48">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
@@ -814,8 +1269,8 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F48">
-      <formula1>$T$4:$T$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G48">
+      <formula1>$U$4:$U$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>